<commit_message>
Added option to remove the worksheet table style.
</commit_message>
<xml_diff>
--- a/test/perl_output/tables.xlsx
+++ b/test/perl_output/tables.xlsx
@@ -19,13 +19,14 @@
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="28">
   <si>
     <t>Default table with no data.</t>
   </si>
@@ -103,6 +104,9 @@
   </si>
   <si>
     <t>Table with alternative Excel style.</t>
+  </si>
+  <si>
+    <t>Table with no Excel style.</t>
   </si>
   <si>
     <t>Table with column formats.</t>
@@ -210,6 +214,23 @@
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="B3:G8" totalsRowCount="1">
+  <autoFilter ref="B3:G7"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Product" totalsRowLabel="Totals"/>
+    <tableColumn id="2" name="Quarter 1" totalsRowFunction="sum"/>
+    <tableColumn id="3" name="Quarter 2" totalsRowFunction="sum"/>
+    <tableColumn id="4" name="Quarter 3" totalsRowFunction="sum"/>
+    <tableColumn id="5" name="Quarter 4" totalsRowFunction="sum"/>
+    <tableColumn id="6" name="Year" totalsRowFunction="sum">
+      <calculatedColumnFormula>SUM(Table12[[#This Row],[Quarter 1]:[Quarter 4]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="B3:G8" totalsRowCount="1">
   <autoFilter ref="B3:G7"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Product" totalsRowLabel="Totals"/>
@@ -1011,6 +1032,159 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>8000</v>
+      </c>
+      <c r="F4">
+        <v>6000</v>
+      </c>
+      <c r="G4">
+        <f>SUM(Table12[[#This Row],[Quarter 1]:[Quarter 4]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="D5">
+        <v>3000</v>
+      </c>
+      <c r="E5">
+        <v>4000</v>
+      </c>
+      <c r="F5">
+        <v>5000</v>
+      </c>
+      <c r="G5">
+        <f>SUM(Table12[[#This Row],[Quarter 1]:[Quarter 4]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>6000</v>
+      </c>
+      <c r="D6">
+        <v>6000</v>
+      </c>
+      <c r="E6">
+        <v>6500</v>
+      </c>
+      <c r="F6">
+        <v>6000</v>
+      </c>
+      <c r="G6">
+        <f>SUM(Table12[[#This Row],[Quarter 1]:[Quarter 4]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7">
+        <v>700</v>
+      </c>
+      <c r="G7">
+        <f>SUM(Table12[[#This Row],[Quarter 1]:[Quarter 4]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <f>SUBTOTAL(109,[Quarter 1])</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>SUBTOTAL(109,[Quarter 2])</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>SUBTOTAL(109,[Quarter 3])</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>SUBTOTAL(109,[Quarter 4])</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>SUBTOTAL(109,[Year])</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="7" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="1">
         <v>10000</v>
       </c>

</xml_diff>